<commit_message>
zed run excel exporter sucks donkey D
</commit_message>
<xml_diff>
--- a/zed_run/overall_horse_stats.xlsx
+++ b/zed_run/overall_horse_stats.xlsx
@@ -135,16 +135,16 @@
         <v>1000.0</v>
       </c>
       <c r="B2" t="n">
-        <v>99108.0</v>
+        <v>101394.0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.449</v>
+        <v>0.45</v>
       </c>
       <c r="D2" t="n">
         <v>50.5892</v>
       </c>
       <c r="E2" t="n">
-        <v>57.21047099931388</v>
+        <v>57.214067598674475</v>
       </c>
       <c r="F2" t="n">
         <v>60.856</v>
@@ -153,16 +153,16 @@
         <v>10.266800000000003</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8676737922178464</v>
+        <v>0.8621410668963386</v>
       </c>
       <c r="I2" t="n">
-        <v>56.689575000000005</v>
+        <v>56.6996</v>
       </c>
       <c r="J2" t="n">
         <v>57.27</v>
       </c>
       <c r="K2" t="n">
-        <v>57.796325</v>
+        <v>57.7947</v>
       </c>
     </row>
     <row r="3">
@@ -170,16 +170,16 @@
         <v>1200.0</v>
       </c>
       <c r="B3" t="n">
-        <v>116460.0</v>
+        <v>118818.0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.421</v>
+        <v>0.422</v>
       </c>
       <c r="D3" t="n">
         <v>63.139</v>
       </c>
       <c r="E3" t="n">
-        <v>70.81727021209</v>
+        <v>70.82140614048376</v>
       </c>
       <c r="F3" t="n">
         <v>75.5047</v>
@@ -188,16 +188,16 @@
         <v>12.365699999999997</v>
       </c>
       <c r="H3" t="n">
-        <v>1.1620355797303905</v>
+        <v>1.1549534660891005</v>
       </c>
       <c r="I3" t="n">
-        <v>70.1268</v>
+        <v>70.13782499999999</v>
       </c>
       <c r="J3" t="n">
-        <v>70.9</v>
+        <v>70.91</v>
       </c>
       <c r="K3" t="n">
-        <v>71.6015</v>
+        <v>71.60027500000001</v>
       </c>
     </row>
     <row r="4">
@@ -205,16 +205,16 @@
         <v>1400.0</v>
       </c>
       <c r="B4" t="n">
-        <v>127995.0</v>
+        <v>130236.0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.396</v>
+        <v>0.398</v>
       </c>
       <c r="D4" t="n">
         <v>70.8811</v>
       </c>
       <c r="E4" t="n">
-        <v>82.92882458221024</v>
+        <v>82.93398855001689</v>
       </c>
       <c r="F4" t="n">
         <v>88.0096</v>
@@ -223,16 +223,16 @@
         <v>17.128500000000003</v>
       </c>
       <c r="H4" t="n">
-        <v>1.4452050993871464</v>
+        <v>1.437473558644611</v>
       </c>
       <c r="I4" t="n">
-        <v>82.07385</v>
+        <v>82.087</v>
       </c>
       <c r="J4" t="n">
-        <v>83.03</v>
+        <v>83.04</v>
       </c>
       <c r="K4" t="n">
-        <v>83.9155</v>
+        <v>83.9138</v>
       </c>
     </row>
     <row r="5">
@@ -240,16 +240,16 @@
         <v>1600.0</v>
       </c>
       <c r="B5" t="n">
-        <v>143400.0</v>
+        <v>145926.0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.391</v>
+        <v>0.392</v>
       </c>
       <c r="D5" t="n">
         <v>82.8611</v>
       </c>
       <c r="E5" t="n">
-        <v>94.99096247559275</v>
+        <v>94.99810640461604</v>
       </c>
       <c r="F5" t="n">
         <v>101.0974</v>
@@ -258,16 +258,16 @@
         <v>18.2363</v>
       </c>
       <c r="H5" t="n">
-        <v>1.6760524951819893</v>
+        <v>1.6673813243137179</v>
       </c>
       <c r="I5" t="n">
-        <v>93.9894</v>
+        <v>94.0064</v>
       </c>
       <c r="J5" t="n">
-        <v>95.12</v>
+        <v>95.13</v>
       </c>
       <c r="K5" t="n">
-        <v>96.1211</v>
+        <v>96.1203</v>
       </c>
     </row>
     <row r="6">
@@ -275,16 +275,16 @@
         <v>1800.0</v>
       </c>
       <c r="B6" t="n">
-        <v>104688.0</v>
+        <v>106725.0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.392</v>
+        <v>0.393</v>
       </c>
       <c r="D6" t="n">
         <v>93.4125</v>
       </c>
       <c r="E6" t="n">
-        <v>107.01747122592847</v>
+        <v>107.0268087917545</v>
       </c>
       <c r="F6" t="n">
         <v>112.9491</v>
@@ -293,16 +293,16 @@
         <v>19.536600000000007</v>
       </c>
       <c r="H6" t="n">
-        <v>1.854646265746837</v>
+        <v>1.8443838565561554</v>
       </c>
       <c r="I6" t="n">
-        <v>105.9121</v>
+        <v>105.9317</v>
       </c>
       <c r="J6" t="n">
-        <v>107.17</v>
+        <v>107.18</v>
       </c>
       <c r="K6" t="n">
-        <v>108.2823</v>
+        <v>108.2829</v>
       </c>
     </row>
     <row r="7">
@@ -310,16 +310,16 @@
         <v>2000.0</v>
       </c>
       <c r="B7" t="n">
-        <v>119571.0</v>
+        <v>121377.0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.398</v>
+        <v>0.399</v>
       </c>
       <c r="D7" t="n">
         <v>104.4713</v>
       </c>
       <c r="E7" t="n">
-        <v>118.90427863612415</v>
+        <v>118.91322819562191</v>
       </c>
       <c r="F7" t="n">
         <v>127.593</v>
@@ -328,16 +328,16 @@
         <v>23.121700000000004</v>
       </c>
       <c r="H7" t="n">
-        <v>2.062414325260168</v>
+        <v>2.0537577044301254</v>
       </c>
       <c r="I7" t="n">
-        <v>117.66335000000001</v>
+        <v>117.6816</v>
       </c>
       <c r="J7" t="n">
-        <v>119.07</v>
+        <v>119.09</v>
       </c>
       <c r="K7" t="n">
-        <v>120.3138</v>
+        <v>120.314</v>
       </c>
     </row>
     <row r="8">
@@ -345,16 +345,16 @@
         <v>2200.0</v>
       </c>
       <c r="B8" t="n">
-        <v>122523.0</v>
+        <v>124758.0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.421</v>
+        <v>0.423</v>
       </c>
       <c r="D8" t="n">
         <v>114.5522</v>
       </c>
       <c r="E8" t="n">
-        <v>130.80292797025865</v>
+        <v>130.81677295804678</v>
       </c>
       <c r="F8" t="n">
         <v>139.1872</v>
@@ -363,16 +363,16 @@
         <v>24.63499999999999</v>
       </c>
       <c r="H8" t="n">
-        <v>2.2762423385822967</v>
+        <v>2.264490349651805</v>
       </c>
       <c r="I8" t="n">
-        <v>129.42835000000002</v>
+        <v>129.4574</v>
       </c>
       <c r="J8" t="n">
-        <v>130.98</v>
+        <v>131.0</v>
       </c>
       <c r="K8" t="n">
-        <v>132.36235</v>
+        <v>132.3659</v>
       </c>
     </row>
     <row r="9">
@@ -380,16 +380,16 @@
         <v>2400.0</v>
       </c>
       <c r="B9" t="n">
-        <v>90825.0</v>
+        <v>92790.0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.458</v>
+        <v>0.46</v>
       </c>
       <c r="D9" t="n">
         <v>126.2645</v>
       </c>
       <c r="E9" t="n">
-        <v>142.56298291990092</v>
+        <v>142.58305632719043</v>
       </c>
       <c r="F9" t="n">
         <v>151.1645</v>
@@ -398,16 +398,16 @@
         <v>24.900000000000006</v>
       </c>
       <c r="H9" t="n">
-        <v>2.541063739586313</v>
+        <v>2.5254528284799864</v>
       </c>
       <c r="I9" t="n">
-        <v>141.0186</v>
+        <v>141.0577</v>
       </c>
       <c r="J9" t="n">
-        <v>142.79</v>
+        <v>142.82</v>
       </c>
       <c r="K9" t="n">
-        <v>144.315</v>
+        <v>144.3197</v>
       </c>
     </row>
     <row r="10">
@@ -415,16 +415,16 @@
         <v>2600.0</v>
       </c>
       <c r="B10" t="n">
-        <v>13887.0</v>
+        <v>14220.0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.492</v>
+        <v>0.494</v>
       </c>
       <c r="D10" t="n">
         <v>135.2961</v>
       </c>
       <c r="E10" t="n">
-        <v>154.33926766040182</v>
+        <v>154.3668159774965</v>
       </c>
       <c r="F10" t="n">
         <v>164.37</v>
@@ -433,16 +433,16 @@
         <v>29.07390000000001</v>
       </c>
       <c r="H10" t="n">
-        <v>2.917400712426944</v>
+        <v>2.8989805076639117</v>
       </c>
       <c r="I10" t="n">
-        <v>152.62045</v>
+        <v>152.6662</v>
       </c>
       <c r="J10" t="n">
-        <v>154.67</v>
+        <v>154.7</v>
       </c>
       <c r="K10" t="n">
-        <v>156.3576</v>
+        <v>156.37052500000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>